<commit_message>
Fix bugs | Href in admin direct in itself | Add more information for admin to type in
</commit_message>
<xml_diff>
--- a/view/admin/hoa-don-nhap-hang.xlsx
+++ b/view/admin/hoa-don-nhap-hang.xlsx
@@ -65,7 +65,7 @@
     <t>Áo Polo Nam Cafe</t>
   </si>
   <si>
-    <t>NCC001</t>
+    <t>NCC00001</t>
   </si>
   <si>
     <t>An Dương - Công Ty TNHH Thương Mại Thời Trang An Dương</t>
@@ -1305,7 +1305,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="7"/>

</xml_diff>